<commit_message>
Exported energy storage scenarios and moved script from folder
</commit_message>
<xml_diff>
--- a/docs/Files/ODYM_Classifications_Master_Vehicle_System.xlsx
+++ b/docs/Files/ODYM_Classifications_Master_Vehicle_System.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E63703-84DC-8E48-840F-9BFE2F6DC654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4BA200-1702-8A42-8E68-D586D7AEA6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="38400" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="306">
   <si>
     <t>Name</t>
   </si>
@@ -13963,10 +13963,10 @@
   <dimension ref="A1:AA1311"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="Q16" sqref="Q16"/>
+      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14576,9 +14576,8 @@
         <f>Ownership_Scenarios!D2</f>
         <v>Low</v>
       </c>
-      <c r="O11" s="13" t="str">
-        <f>Energy_Storage_Scenarios!D2</f>
-        <v>IRENA_ref_high</v>
+      <c r="O11" s="13" t="s">
+        <v>281</v>
       </c>
       <c r="P11" s="7" t="str">
         <f>V2G_Scenarios!D2</f>
@@ -14633,9 +14632,8 @@
         <f>Ownership_Scenarios!D3</f>
         <v>BAU</v>
       </c>
-      <c r="O12" s="13" t="str">
-        <f>Energy_Storage_Scenarios!D3</f>
-        <v>IRENA_remap_high</v>
+      <c r="O12" s="13" t="s">
+        <v>277</v>
       </c>
       <c r="P12" s="7" t="str">
         <f>V2G_Scenarios!D3</f>
@@ -14689,7 +14687,9 @@
         <f>Ownership_Scenarios!D4</f>
         <v>High</v>
       </c>
-      <c r="O13" s="13"/>
+      <c r="O13" s="13" t="s">
+        <v>280</v>
+      </c>
       <c r="P13" s="7" t="str">
         <f>V2G_Scenarios!D4</f>
         <v>High</v>

</xml_diff>

<commit_message>
Added scenarios and plots
</commit_message>
<xml_diff>
--- a/docs/Files/ODYM_Classifications_Master_Vehicle_System.xlsx
+++ b/docs/Files/ODYM_Classifications_Master_Vehicle_System.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0692F95-3CE7-F440-9051-2CDBB3B18D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ED81AA-CE50-EA43-90A4-60D7BEE6B783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="38400" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13981,10 +13981,10 @@
   <dimension ref="A1:AA1311"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14683,10 +14683,6 @@
       <c r="I13" s="7" t="str">
         <f>Recycling_Process!D4</f>
         <v>Pyrometallurgy</v>
-      </c>
-      <c r="J13" s="7" t="str">
-        <f>EV_penetration_scenario!D4</f>
-        <v>Net Zero</v>
       </c>
       <c r="K13" s="7" t="str">
         <f>Size!D4</f>

</xml_diff>

<commit_message>
Worked on SLB appproach and plots
</commit_message>
<xml_diff>
--- a/docs/Files/ODYM_Classifications_Master_Vehicle_System.xlsx
+++ b/docs/Files/ODYM_Classifications_Master_Vehicle_System.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95AD7FC-38D7-FC43-A1F9-21D44AA92A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEE359E-12FA-6442-9BCB-6646300BB40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="38400" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="316">
   <si>
     <t>Name</t>
   </si>
@@ -1003,6 +1003,12 @@
   </si>
   <si>
     <t>No reuse</t>
+  </si>
+  <si>
+    <t>Slow EV</t>
+  </si>
+  <si>
+    <t>Fast EV</t>
   </si>
 </sst>
 </file>
@@ -13987,10 +13993,10 @@
   <dimension ref="A1:AA1311"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14581,9 +14587,8 @@
         <f>Recycling_Process!D2</f>
         <v>Direct</v>
       </c>
-      <c r="J11" s="7" t="str">
-        <f>EV_penetration_scenario!D2</f>
-        <v>STEP</v>
+      <c r="J11" s="7" t="s">
+        <v>314</v>
       </c>
       <c r="K11" s="7" t="str">
         <f>Size!D2</f>
@@ -14634,9 +14639,8 @@
         <f>Recycling_Process!D3</f>
         <v>Hydrometallurgy</v>
       </c>
-      <c r="J12" s="7" t="str">
-        <f>EV_penetration_scenario!D3</f>
-        <v>SD</v>
+      <c r="J12" s="7" t="s">
+        <v>315</v>
       </c>
       <c r="K12" s="7" t="str">
         <f>Size!D3</f>

</xml_diff>